<commit_message>
three graphs were deleted
</commit_message>
<xml_diff>
--- a/enterData/table.xlsx
+++ b/enterData/table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Саморазвитие\Программирование\Python course\conflictMath\enterData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A8A0FB-0CDC-4E4D-975A-F8F5A7E642F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F7B003-F212-4962-B7D7-5C84F03122F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="2220" windowWidth="17280" windowHeight="8964" xr2:uid="{7D3AC649-DD75-434C-A112-F2107D6B7801}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7D3AC649-DD75-434C-A112-F2107D6B7801}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -49,6 +49,63 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -474,15 +531,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A959C7E2-B3CA-4640-8976-7D4701CD0023}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -498,8 +555,65 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -509,14 +623,71 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -530,10 +701,67 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -549,8 +777,65 @@
       <c r="E4" s="2">
         <v>0</v>
       </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V4" s="2">
+        <v>0</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -564,10 +849,67 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -578,13 +920,70 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -595,13 +994,70 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R7" s="2">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -615,10 +1071,67 @@
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -628,14 +1141,71 @@
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>4</v>
+      <c r="D9" s="2">
+        <v>0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V9" s="2">
+        <v>0</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -646,13 +1216,70 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -662,14 +1289,71 @@
       <c r="C11" s="2">
         <v>0</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W11" s="2">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -680,13 +1364,70 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X12" s="2">
+        <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -696,11 +1437,68 @@
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>2</v>
+      <c r="D13" s="2">
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>